<commit_message>
corrections aphid trait import
</commit_message>
<xml_diff>
--- a/data/Checklist 2020_maud edits.xlsx
+++ b/data/Checklist 2020_maud edits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maud/Dropbox/Work/doc boulot/postdoc Berlin/R projects/AphidTraits/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85483D31-4C75-F84A-9918-91C524AB292A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5338AE77-6995-2441-BFA9-18E03BBC4913}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" firstSheet="1" activeTab="6" xr2:uid="{83007F86-AA6F-4A3C-9AE4-7210E3AB2052}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{83007F86-AA6F-4A3C-9AE4-7210E3AB2052}"/>
   </bookViews>
   <sheets>
     <sheet name="Oh_01" sheetId="1" r:id="rId1"/>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF0A5DB-A781-4832-96C4-9796ADDFE949}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="217" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8472,8 +8472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF24A4C9-C359-4164-A5A2-173E182EBAB7}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>